<commit_message>
-updates to energy help
-correct electric co2 conversion value
-remove debug prints
</commit_message>
<xml_diff>
--- a/doc/help_dialogs/Input_files/energy.xlsx
+++ b/doc/help_dialogs/Input_files/energy.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Intro" sheetId="1" r:id="rId1"/>
@@ -78,9 +78,6 @@
     <t>Between Batches after Pre-Heating</t>
   </si>
   <si>
-    <t xml:space="preserve">tn:Begin by making entries on the Loads tab.  </t>
-  </si>
-  <si>
     <t>tn:Power ratings for up to four energy loads may be entered.  Loads will be the main burners or heaters, motors and blowers, and the afterburner if one is used.  Enter one load per line.  Motors and blowers that run continuously may be aggregated and entered as one load.</t>
   </si>
   <si>
@@ -96,9 +93,6 @@
     <t>When an Event is selected in the previous column this value can be set to match the 0% burner setting to the event setting.  In most cases a 0 Event value will correspond to the 0% load setting.</t>
   </si>
   <si>
-    <t xml:space="preserve">When an Event is selected this value can be set to match the 100% load setting to the event setting.  This is useful when the 100% load setting is recorded as a different number in the Event.  For instance, maybe the burner event is recorded as 10x the kPa reading on the gas manometer.  An event value of 30 is recoded to signify 3 kPa.  If the 100% burner setting corresponds to 7 kPa then the 'Value 100%' should be set to 60, which is 7 * 10  = 70.  </t>
-  </si>
-  <si>
     <t>Pressure %</t>
   </si>
   <si>
@@ -126,9 +120,6 @@
     <t>This setting allows to set a mix of renewable energy that sources the electric loads.  0% assumes all the energy comes from burning dirty coal and maximizes the CO2 in the calculations.  100% assumes the energy comes only from renewable sources with no CO2 produced.</t>
   </si>
   <si>
-    <t>Save as Defaults</t>
-  </si>
-  <si>
     <t>Restore Defaults</t>
   </si>
   <si>
@@ -168,9 +159,6 @@
     <t>tn:To use the Artisan energy measurement feature you will need to record one or more profiles that include the protocol of interest.  For example, to measure the Pre-Heating energy, START recording when the roaster is turned on.  Let Artisan record the entire pre-heating procedure.  At the end of the pre-heating you can either STOP recording the profile or go forward with the roast.  The CHARGE event will mark the end of pre-heating when Artisan measures the pre-heat energy.  Similarly a Between Batches protocol can be recorded with START followed by a normal roast.  A Cooling protocol would be captured by not turning the Artisan recording OFF until the roaster is fully cooled.</t>
   </si>
   <si>
-    <t>This row sets the values for between batches protocol for the roasting session.  Percentage or measured values may be entered for each burner.  When a percentage is used the Duration field must be set.\n\nBetween Batches energy is applied to each batch of the roasting session, except the first batch.  Tick the 'Between Batches after Pre-Heating' box to apply Between Batches energies to the first batch of the session.</t>
-  </si>
-  <si>
     <t>Energy is measured from the open profile for each load where an event is specified on the Loads tab.  Click OK to auto fill in the associated Measured Energy field.</t>
   </si>
   <si>
@@ -187,13 +175,25 @@
   </si>
   <si>
     <t>tn:This tab shows a detailed table of the energy consumption and CO2 production data for the roast.  The values in this table are based on current Profile and the settings made on the Loads and Protocols tabs.  Columns may be sorted by clicking on the column title.  To return to original sort click on the 'Kind' column title.</t>
+  </si>
+  <si>
+    <t>When an Event is selected this value can be set to match the 100% load setting to the event setting.  This is useful when the 100% load setting is recorded as a different number in the Event.  For instance, maybe the burner event is recorded as 10x the kPa reading on the gas manometer.  An event value of 35 is recoded to signify 3.5 kPa, which is 50% pressure.  If the 100% burner setting corresponds to 7 kPa then the 'Value 100%' should be set to 70, which is 7 * 10  = 70.  Thus 3.5 kPa will be seen by he energy calculator as 50%.  For pressure readings be sure to tick the Pressure box.  Heat energy readings are normally 0%-100% and do not require any adjustment to this  setting.</t>
+  </si>
+  <si>
+    <t>This row sets the values for between batches protocol for the roasting session.  Percentage or measured values may be entered for each burner.  When a percentage is used the Duration field must be set.\n\nBetween Batches energy is applied to each batch of the roasting session, except the first batch.  Tick the 'Between Batches after Pre-Heating' box to apply Between Batches energies to the first batch of the session too.</t>
+  </si>
+  <si>
+    <t>tn:Begin by making entries on the Loads tab  to define the sources of energy used by this roast. It might be a good idea to save those settings as defaults to be used to calculate the energy consumption of future roasts</t>
+  </si>
+  <si>
+    <t>Save Defaults</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -205,6 +205,13 @@
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial Unicode MS"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
     </font>
@@ -229,7 +236,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -238,6 +245,8 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -557,7 +566,7 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
@@ -582,7 +591,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -590,12 +599,12 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
     </row>
   </sheetData>
@@ -608,8 +617,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B20"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -620,12 +629,12 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>18</v>
+      <c r="A2" s="5" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -635,7 +644,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -645,7 +654,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -655,7 +664,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -679,7 +688,7 @@
         <v>5</v>
       </c>
       <c r="B11" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
@@ -687,7 +696,7 @@
         <v>6</v>
       </c>
       <c r="B12" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
@@ -695,7 +704,7 @@
         <v>7</v>
       </c>
       <c r="B13" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
@@ -703,15 +712,15 @@
         <v>8</v>
       </c>
       <c r="B14" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B15" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
@@ -719,7 +728,7 @@
         <v>9</v>
       </c>
       <c r="B16" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
@@ -727,31 +736,31 @@
         <v>10</v>
       </c>
       <c r="B17" t="s">
-        <v>24</v>
+        <v>51</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B18" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>34</v>
+        <v>54</v>
       </c>
       <c r="B19" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B20" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -765,7 +774,7 @@
   <dimension ref="A1:B19"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -776,12 +785,12 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -791,7 +800,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -801,7 +810,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -811,7 +820,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -824,10 +833,10 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>26</v>
+      </c>
+      <c r="B10" t="s">
         <v>28</v>
-      </c>
-      <c r="B10" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -835,15 +844,15 @@
         <v>12</v>
       </c>
       <c r="B11" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B12" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
@@ -864,10 +873,10 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B15" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
@@ -875,35 +884,35 @@
         <v>17</v>
       </c>
       <c r="B16" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>34</v>
+      <c r="A17" s="4" t="s">
+        <v>54</v>
       </c>
       <c r="B17" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B18" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B19" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
fix energy protocol percent entry issue
</commit_message>
<xml_diff>
--- a/doc/help_dialogs/Input_files/energy.xlsx
+++ b/doc/help_dialogs/Input_files/energy.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="20730" windowHeight="11760" tabRatio="500"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="20730" windowHeight="11760" tabRatio="500" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Intro" sheetId="1" r:id="rId1"/>
@@ -114,15 +114,9 @@
     <t>Pre-Heating</t>
   </si>
   <si>
-    <t>tn:The Protocol settings allow including Pre-Heating, Between Batch (BBP) and Cooling protocol energy consumption.  There are two ways to specify these values.  The first assumes a constant load setting for a defined period of time.  An example for Preheating is to set a Duration of 45:00 (45 minutes) at 30% Burner setting.  Percentages may be entered either as a decimal (.30) or a percentage (30%).  When a percentage is entered  a corresponding Duration must be entered.</t>
-  </si>
-  <si>
     <t>This row sets the values for pre-heating energy.  Percentage or measured values may be entered for each burner.  When a percentage is used the Duration field must be set.\n\nPre-Heating energy is applied only to the first batch of a roasting session.</t>
   </si>
   <si>
-    <t>This box should be ticked when a Between Batches protocol run is done after the Preheating and before the roast.</t>
-  </si>
-  <si>
     <t>Electric Energy Mix</t>
   </si>
   <si>
@@ -135,9 +129,6 @@
     <t>Results in</t>
   </si>
   <si>
-    <t>tn:The Energy tab displays a roast's energy consumption.   CO2 emissions are also calculated to monitor the impact of the roasting operation.  Settings must be made for each energy load.  Loads are the main burners, motors and blowers, and an afterburner if one is used.  The energy used for preheating, between batch, and roaster cooling protocols are included in the calculations, and settings are available for them as well.\n\nNote that pre-heating and roaster cooling energy values are applied to the first roast of a roasting session.  Between batch energies are applied to every roast except the first.  Tick the "Between batches after Pre-Heating box to apply the between batch value to the first roast.\n\nFollow the steps below to set the energy inputs for the roast machine and afterburner.</t>
-  </si>
-  <si>
     <t>Measure Profile […]</t>
   </si>
   <si>
@@ -202,6 +193,15 @@
   </si>
   <si>
     <t>bn:Once you set up the Loads sub-tab and the Protocols sub-tab, it is a good idea to click "Save Defaults" on both  sub-tabs (they are saved separately).  When loading a profile with existing energy values, the profile settings will be read and will overwrite the values on the Loads and Profiles sub-tabs.  Having them saved as defaults allow for them to be quickly restored by clicking "Restore Defaults" on each sub-tab.</t>
+  </si>
+  <si>
+    <t>tn:The Energy tab displays a roast's energy consumption.   CO2 emissions are also calculated to monitor the impact of the roasting operation.  Settings must be made for each energy load.  Loads are the main burners, motors and blowers, and an afterburner if one is used.  The energy used for pre-heating, between batch, and roaster cooling protocols are included in the calculations, and settings are available for them as well.\n\nNote that pre-heating and roaster cooling energy values are applied to the first roast of a roasting session.  Between batch energies are applied to every roast except the first.  Tick the "Between batches after Pre-Heating box to apply the between batch value to the first roast.\n\nFollow the steps below to set the energy inputs for the roast machine and afterburner.</t>
+  </si>
+  <si>
+    <t>This box should be ticked when a Between Batches protocol run is done after the Pre-heating and before the roast.</t>
+  </si>
+  <si>
+    <t>tn:The Protocol settings allow including Pre-Heating, Between Batch (BBP) and Cooling protocol energy consumption.  There are two ways to specify these values.  The first assumes a constant load setting for a defined period of time.  An example for pre-heating is to set a Duration of 45:00 (45 minutes) at 30% Burner setting.  Percentages must be entered with the percent sign (30%).  When a percentage is entered  a corresponding Duration must be entered.</t>
   </si>
 </sst>
 </file>
@@ -558,10 +558,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A10"/>
+  <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -569,41 +569,42 @@
     <col min="1" max="1" width="37.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B7" s="1"/>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
     </row>
   </sheetData>
@@ -617,19 +618,19 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -642,10 +643,10 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B4" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
   </sheetData>
@@ -670,12 +671,12 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -705,7 +706,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -737,7 +738,7 @@
         <v>6</v>
       </c>
       <c r="B12" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
@@ -753,7 +754,7 @@
         <v>8</v>
       </c>
       <c r="B14" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
@@ -777,31 +778,31 @@
         <v>10</v>
       </c>
       <c r="B17" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B18" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B19" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B20" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
     </row>
   </sheetData>
@@ -814,8 +815,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B18"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -826,12 +827,12 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>27</v>
+        <v>56</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -841,7 +842,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -851,7 +852,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -861,7 +862,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -877,7 +878,7 @@
         <v>26</v>
       </c>
       <c r="B10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -885,7 +886,7 @@
         <v>12</v>
       </c>
       <c r="B11" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
@@ -893,7 +894,7 @@
         <v>25</v>
       </c>
       <c r="B12" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
@@ -914,10 +915,10 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
+        <v>32</v>
+      </c>
+      <c r="B15" t="s">
         <v>35</v>
-      </c>
-      <c r="B15" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
@@ -925,23 +926,23 @@
         <v>17</v>
       </c>
       <c r="B16" t="s">
-        <v>29</v>
+        <v>55</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B17" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B18" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
adds meter settings to energy help
</commit_message>
<xml_diff>
--- a/doc/help_dialogs/Input_files/energy.xlsx
+++ b/doc/help_dialogs/Input_files/energy.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28429"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dave\Documents\GitHub\artisan\doc\help_dialogs\Input_files\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1032B0DB-A399-491A-9C9D-8BDFF7717BB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="20730" windowHeight="11760" tabRatio="500" activeTab="3"/>
+    <workbookView xWindow="900" yWindow="330" windowWidth="17430" windowHeight="10790" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Intro" sheetId="1" r:id="rId1"/>
@@ -12,17 +18,8 @@
     <sheet name="Loads" sheetId="2" r:id="rId3"/>
     <sheet name="Protocol" sheetId="3" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="145621" iterateDelta="1E-4"/>
   <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
     </ext>
@@ -31,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="70">
   <si>
     <t>Energy and CO2 Calculator</t>
   </si>
@@ -202,13 +199,52 @@
   </si>
   <si>
     <t>tn:The Protocol settings allow including Pre-Heating, Between Batch (BBP) and Cooling protocol energy consumption.  There are two ways to specify these values.  The first assumes a constant load setting for a defined period of time.  An example for pre-heating is to set a Duration of 45:00 (45 minutes) at 30% Burner setting.  Percentages must be entered with the percent sign (30%).  When a percentage is entered  a corresponding Duration must be entered.</t>
+  </si>
+  <si>
+    <t>tn:Energy Meters</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tn:Artisan allows the direct reading of 2 energy meters to support the use of measured energy consumption values in place of estimated values defined by the Loads. These energy meters could measure gas or electricity. As an energy meter the instantaneous power reading must be accumulated over a period of time.  Energy readings are typically in kWh or BTU, though other units are supported.  Artisan will use the Meter reading at the start of recording and end of recording to calculate energy consumption for the roast batch.  Intermediate reads at major roast events are also used in presenting phase energy consumption.  </t>
+  </si>
+  <si>
+    <t>Meter Label</t>
+  </si>
+  <si>
+    <t>Meter Unit</t>
+  </si>
+  <si>
+    <t>Meter Type</t>
+  </si>
+  <si>
+    <t>Gas Energy Mix</t>
+  </si>
+  <si>
+    <t>This setting allows to set a mix of bio gas in the NG source.  0% thus means no bio gas.  100% bio gas is estimated to reduce GHG emissions by approximately 24%.</t>
+  </si>
+  <si>
+    <t>A user defined label for the meter.</t>
+  </si>
+  <si>
+    <t>Meter Source</t>
+  </si>
+  <si>
+    <t>The type of fuel measured by this meter.</t>
+  </si>
+  <si>
+    <t>The Extra Device holding the scaled energy data.</t>
+  </si>
+  <si>
+    <t>The energy unit for the data read from the Extra Device.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tn:Energy meter data must be recorded in an Extra Device (Config&gt;&gt; Devices&gt;&gt; Extra devices tab).  The Extra Device is then used as the Source for the meter in the Energy tab.  Connectivity to the meter is typically via MODBUS. Some devices, like the YoctoWatt, have direct connection support in Artisan.  The data recorded in the Extra Device must be scaled to one of the units supported in the Energy tab such as kWh, BTU, kJ, kCal or therms (thm).  For instance, an electricity meter that returns energy readings in Wh that must be scaled to kWh buy using the symbolic equation "x/1000". </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -244,16 +280,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -272,9 +306,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -312,7 +346,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -384,7 +418,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -557,54 +591,52 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="37.28515625" customWidth="1"/>
+    <col min="1" max="1" width="37.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2">
       <c r="A3" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2">
       <c r="A4" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2">
       <c r="A5" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2">
       <c r="A8" s="1"/>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2">
       <c r="A9" s="1"/>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2">
       <c r="A10" s="1"/>
     </row>
   </sheetData>
@@ -614,26 +646,26 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.5"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -641,7 +673,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2">
       <c r="A4" t="s">
         <v>31</v>
       </c>
@@ -656,152 +688,217 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B20"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:B30"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="43.140625" customWidth="1"/>
-    <col min="2" max="2" width="62.5703125" customWidth="1"/>
+    <col min="1" max="1" width="43.1796875" customWidth="1"/>
+    <col min="2" max="2" width="62.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2">
       <c r="A3" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2">
       <c r="A4" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2">
       <c r="A5" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2">
       <c r="A6" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2">
       <c r="A7" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2">
       <c r="A8" s="1" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+    <row r="9" spans="1:2">
+      <c r="A9" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14" t="s">
         <v>1</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B14" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+    <row r="15" spans="1:2">
+      <c r="A15" t="s">
         <v>3</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B15" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+    <row r="16" spans="1:2">
+      <c r="A16" t="s">
         <v>5</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B16" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+    <row r="17" spans="1:2">
+      <c r="A17" t="s">
         <v>6</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B17" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+    <row r="18" spans="1:2">
+      <c r="A18" t="s">
         <v>7</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B18" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+    <row r="19" spans="1:2">
+      <c r="A19" t="s">
         <v>8</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B19" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+    <row r="20" spans="1:2">
+      <c r="A20" t="s">
         <v>23</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B20" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+    <row r="21" spans="1:2">
+      <c r="A21" t="s">
         <v>9</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B21" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+    <row r="22" spans="1:2">
+      <c r="A22" t="s">
         <v>10</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B22" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+    <row r="23" spans="1:2">
+      <c r="A23" t="s">
+        <v>59</v>
+      </c>
+      <c r="B23" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2">
+      <c r="A24" t="s">
+        <v>60</v>
+      </c>
+      <c r="B24" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2">
+      <c r="A25" t="s">
+        <v>61</v>
+      </c>
+      <c r="B25" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2">
+      <c r="A26" t="s">
+        <v>65</v>
+      </c>
+      <c r="B26" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2">
+      <c r="A27" t="s">
         <v>28</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B27" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+    <row r="28" spans="1:2">
+      <c r="A28" t="s">
+        <v>62</v>
+      </c>
+      <c r="B28" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2">
+      <c r="A29" t="s">
         <v>41</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B29" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+    <row r="30" spans="1:2">
+      <c r="A30" t="s">
         <v>30</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B30" t="s">
         <v>51</v>
       </c>
     </row>
@@ -812,60 +909,60 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:B18"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="31.28515625" customWidth="1"/>
+    <col min="1" max="1" width="31.26953125" customWidth="1"/>
     <col min="2" max="2" width="38" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
+    <row r="4" spans="1:2">
+      <c r="A4" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2">
       <c r="A5" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2">
       <c r="A6" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2">
       <c r="A7" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2">
       <c r="A8" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2">
       <c r="A9" t="s">
         <v>1</v>
       </c>
@@ -873,7 +970,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2">
       <c r="A10" t="s">
         <v>26</v>
       </c>
@@ -881,7 +978,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2">
       <c r="A11" t="s">
         <v>12</v>
       </c>
@@ -889,7 +986,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2">
       <c r="A12" t="s">
         <v>25</v>
       </c>
@@ -897,7 +994,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2">
       <c r="A13" t="s">
         <v>13</v>
       </c>
@@ -905,7 +1002,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2">
       <c r="A14" t="s">
         <v>15</v>
       </c>
@@ -913,7 +1010,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2">
       <c r="A15" t="s">
         <v>32</v>
       </c>
@@ -921,7 +1018,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2">
       <c r="A16" t="s">
         <v>17</v>
       </c>
@@ -929,7 +1026,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2">
       <c r="A17" t="s">
         <v>41</v>
       </c>
@@ -937,7 +1034,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2">
       <c r="A18" t="s">
         <v>30</v>
       </c>

</xml_diff>